<commit_message>
Updates as part of finishing up the diversity metrics.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientNames_Units.xlsx
+++ b/data-raw/NutrientData/nutrientNames_Units.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="112">
   <si>
     <t>edible_share</t>
   </si>
@@ -357,6 +357,12 @@
   </si>
   <si>
     <t>Retention code</t>
+  </si>
+  <si>
+    <t>phytate_source</t>
+  </si>
+  <si>
+    <t>Source of phytate info</t>
   </si>
 </sst>
 </file>
@@ -749,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA3"/>
+  <dimension ref="A1:BB3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -761,47 +767,47 @@
     <col min="3" max="4" width="18.6640625" customWidth="1"/>
     <col min="5" max="5" width="44.6640625" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" customWidth="1"/>
-    <col min="9" max="9" width="27.6640625" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" customWidth="1"/>
-    <col min="13" max="13" width="8.6640625" customWidth="1"/>
-    <col min="14" max="15" width="13.6640625" customWidth="1"/>
-    <col min="16" max="16" width="12.6640625" customWidth="1"/>
-    <col min="17" max="17" width="8.6640625" customWidth="1"/>
-    <col min="18" max="18" width="30.6640625" customWidth="1"/>
-    <col min="19" max="19" width="10.6640625" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" customWidth="1"/>
-    <col min="21" max="21" width="9.6640625" customWidth="1"/>
-    <col min="22" max="23" width="11.6640625" customWidth="1"/>
-    <col min="24" max="24" width="12.6640625" customWidth="1"/>
-    <col min="25" max="25" width="14.6640625" customWidth="1"/>
-    <col min="26" max="26" width="28.6640625" customWidth="1"/>
-    <col min="27" max="27" width="19.6640625" customWidth="1"/>
-    <col min="28" max="28" width="25.6640625" customWidth="1"/>
-    <col min="29" max="30" width="28.6640625" customWidth="1"/>
-    <col min="31" max="33" width="34.6640625" customWidth="1"/>
-    <col min="34" max="34" width="14.6640625" customWidth="1"/>
-    <col min="35" max="35" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.6640625" customWidth="1"/>
-    <col min="37" max="38" width="10.6640625" customWidth="1"/>
-    <col min="39" max="39" width="25.6640625" customWidth="1"/>
-    <col min="40" max="40" width="26.6640625" customWidth="1"/>
-    <col min="41" max="41" width="28.6640625" customWidth="1"/>
-    <col min="42" max="42" width="24.6640625" customWidth="1"/>
-    <col min="43" max="44" width="28.6640625" customWidth="1"/>
-    <col min="45" max="45" width="25.6640625" customWidth="1"/>
-    <col min="46" max="46" width="22.6640625" customWidth="1"/>
-    <col min="47" max="47" width="25.6640625" customWidth="1"/>
-    <col min="48" max="49" width="27.6640625" customWidth="1"/>
-    <col min="50" max="50" width="29.6640625" customWidth="1"/>
-    <col min="51" max="51" width="31.6640625" customWidth="1"/>
-    <col min="52" max="53" width="28.6640625" customWidth="1"/>
+    <col min="7" max="8" width="9.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" customWidth="1"/>
+    <col min="15" max="16" width="13.6640625" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" customWidth="1"/>
+    <col min="18" max="18" width="8.6640625" customWidth="1"/>
+    <col min="19" max="19" width="30.6640625" customWidth="1"/>
+    <col min="20" max="20" width="10.6640625" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" customWidth="1"/>
+    <col min="22" max="22" width="9.6640625" customWidth="1"/>
+    <col min="23" max="24" width="11.6640625" customWidth="1"/>
+    <col min="25" max="25" width="12.6640625" customWidth="1"/>
+    <col min="26" max="26" width="14.6640625" customWidth="1"/>
+    <col min="27" max="27" width="28.6640625" customWidth="1"/>
+    <col min="28" max="28" width="19.6640625" customWidth="1"/>
+    <col min="29" max="29" width="25.6640625" customWidth="1"/>
+    <col min="30" max="31" width="28.6640625" customWidth="1"/>
+    <col min="32" max="34" width="34.6640625" customWidth="1"/>
+    <col min="35" max="35" width="14.6640625" customWidth="1"/>
+    <col min="36" max="36" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="24.6640625" customWidth="1"/>
+    <col min="38" max="39" width="10.6640625" customWidth="1"/>
+    <col min="40" max="40" width="25.6640625" customWidth="1"/>
+    <col min="41" max="41" width="26.6640625" customWidth="1"/>
+    <col min="42" max="42" width="28.6640625" customWidth="1"/>
+    <col min="43" max="43" width="24.6640625" customWidth="1"/>
+    <col min="44" max="45" width="28.6640625" customWidth="1"/>
+    <col min="46" max="46" width="25.6640625" customWidth="1"/>
+    <col min="47" max="47" width="22.6640625" customWidth="1"/>
+    <col min="48" max="48" width="25.6640625" customWidth="1"/>
+    <col min="49" max="50" width="27.6640625" customWidth="1"/>
+    <col min="51" max="51" width="29.6640625" customWidth="1"/>
+    <col min="52" max="52" width="31.6640625" customWidth="1"/>
+    <col min="53" max="54" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -823,146 +829,149 @@
       <c r="G1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>17</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>18</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>7</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>26</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>27</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>28</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AL1" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>103</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>41</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>42</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>46</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>32</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>34</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>35</v>
       </c>
-      <c r="AX1" s="6" t="s">
+      <c r="AY1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>33</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>39</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>105</v>
       </c>
@@ -976,146 +985,149 @@
       <c r="G2" t="s">
         <v>108</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AO2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="AP2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AP2" s="1" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="BA2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="BA2" s="1" t="s">
+      <c r="BB2" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>92</v>
       </c>
@@ -1125,9 +1137,6 @@
       <c r="G3" t="s">
         <v>95</v>
       </c>
-      <c r="H3" t="s">
-        <v>94</v>
-      </c>
       <c r="I3" t="s">
         <v>94</v>
       </c>
@@ -1137,12 +1146,12 @@
       <c r="K3" t="s">
         <v>94</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" t="s">
+        <v>94</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="M3" t="s">
-        <v>95</v>
-      </c>
       <c r="N3" t="s">
         <v>95</v>
       </c>
@@ -1153,11 +1162,11 @@
         <v>95</v>
       </c>
       <c r="Q3" t="s">
+        <v>95</v>
+      </c>
+      <c r="R3" t="s">
         <v>94</v>
       </c>
-      <c r="R3" t="s">
-        <v>95</v>
-      </c>
       <c r="S3" t="s">
         <v>95</v>
       </c>
@@ -1174,7 +1183,7 @@
         <v>95</v>
       </c>
       <c r="X3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y3" t="s">
         <v>96</v>
@@ -1183,16 +1192,16 @@
         <v>96</v>
       </c>
       <c r="AA3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AB3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AC3" t="s">
         <v>96</v>
       </c>
       <c r="AD3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="AE3" t="s">
         <v>94</v>
@@ -1207,13 +1216,13 @@
         <v>94</v>
       </c>
       <c r="AI3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AJ3" t="s">
         <v>95</v>
       </c>
-      <c r="AM3" t="s">
-        <v>104</v>
+      <c r="AK3" t="s">
+        <v>95</v>
       </c>
       <c r="AN3" t="s">
         <v>104</v>
@@ -1255,6 +1264,9 @@
         <v>104</v>
       </c>
       <c r="BA3" t="s">
+        <v>104</v>
+      </c>
+      <c r="BB3" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>